<commit_message>
main translations.xlsx file update
</commit_message>
<xml_diff>
--- a/src/shared/consts/translations.xlsx
+++ b/src/shared/consts/translations.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="1976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="2042">
   <si>
     <t>information_block.literature_text_3</t>
   </si>
@@ -5946,6 +5946,204 @@
   </si>
   <si>
     <t>Within each level, the journey is segmented into four key quadrants - Personal Growth, Friendship, Communication &amp; Conflict, and Dreams. These quadrants are the pillars that support a healthy, thriving relationship, addressing the essential areas for development and understanding.</t>
+  </si>
+  <si>
+    <t>common._each_session</t>
+  </si>
+  <si>
+    <t>*Jede Sitzung schliesst mit einer Challenge ab, betrachtet Sie als eine Art Hausaufgabe oder als ein neues Werkzeug, dass ihr in Zukunft benutzen könnt.</t>
+  </si>
+  <si>
+    <t>*Each session concludes with a challenge, think of it as a homework assignment or a new tool you can use in the future.</t>
+  </si>
+  <si>
+    <t>*Cada sessão termina com um desafio, pense nele como uma tarefa de casa ou uma nova ferramenta que você poderá usar no futuro.</t>
+  </si>
+  <si>
+    <t>sessions.questions_in_sessions_are_on</t>
+  </si>
+  <si>
+    <t>Der Fokus der Fragen in dieser Sitzung liegt auf</t>
+  </si>
+  <si>
+    <t>The focus of the questions in this sessions are on</t>
+  </si>
+  <si>
+    <t>O foco das questões nesta sessão está em</t>
+  </si>
+  <si>
+    <t>sessions.a_handpicked_challenge_is_part_1</t>
+  </si>
+  <si>
+    <t>Eine Auswahl an ausgewählten Core - Challenges der Kategorie Übung</t>
+  </si>
+  <si>
+    <t>A set of handpicked Core - Challenges of the category Exercise</t>
+  </si>
+  <si>
+    <t>Um conjunto de Desafios Core cuidadosamente selecionados da categoria Exercício</t>
+  </si>
+  <si>
+    <t>sessions.a_handpicked_challenge_is_part_2</t>
+  </si>
+  <si>
+    <t>rundet das Bild ab.</t>
+  </si>
+  <si>
+    <t>is rounding up the picture.</t>
+  </si>
+  <si>
+    <t>está completando o quadro.</t>
+  </si>
+  <si>
+    <t>sessions.picked_special_challenge_part_1</t>
+  </si>
+  <si>
+    <t>Die besonderen Herausforderungen in dieser Session:</t>
+  </si>
+  <si>
+    <t>The Special Challenges in this session:</t>
+  </si>
+  <si>
+    <t>Os desafios especiais nesta sessão:</t>
+  </si>
+  <si>
+    <t>therapists.programs_offered_by</t>
+  </si>
+  <si>
+    <t>Programme angeboten von</t>
+  </si>
+  <si>
+    <t>Programs offered by</t>
+  </si>
+  <si>
+    <t>Programas oferecidos por</t>
+  </si>
+  <si>
+    <t>therapists.contacts</t>
+  </si>
+  <si>
+    <t>Kontakte</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Contatos</t>
+  </si>
+  <si>
+    <t>therapist.contact_linkedin</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>therapist.contact_phone</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>therapist.contact_website</t>
+  </si>
+  <si>
+    <t>Webseite</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>therapist.contact_email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>therapist.contact_instagram</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>therapist.contact_youtube</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>languages.en</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>languages.de</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>languages.pt</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>languages.es</t>
+  </si>
+  <si>
+    <t>Spanisch</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Espanhol</t>
+  </si>
+  <si>
+    <t>languages.fr</t>
+  </si>
+  <si>
+    <t>Französisch</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Francês</t>
+  </si>
+  <si>
+    <t>languages.sv</t>
+  </si>
+  <si>
+    <t>Schwedisch</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>Sueco</t>
+  </si>
+  <si>
+    <t>languages.gr</t>
+  </si>
+  <si>
+    <t>Griechisch</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Grego</t>
   </si>
 </sst>
 </file>
@@ -6028,7 +6226,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6068,6 +6266,7 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -14182,31 +14381,286 @@
       </c>
     </row>
     <row r="516" ht="12.75" customHeight="1">
-      <c r="A516" s="1"/>
-      <c r="B516" s="1"/>
-      <c r="C516" s="2"/>
-      <c r="D516" s="1"/>
-      <c r="E516" s="2"/>
-    </row>
-    <row r="517" ht="12.75" customHeight="1"/>
-    <row r="518" ht="12.75" customHeight="1"/>
-    <row r="519" ht="12.75" customHeight="1"/>
-    <row r="520" ht="12.75" customHeight="1"/>
-    <row r="521" ht="12.75" customHeight="1"/>
-    <row r="522" ht="12.75" customHeight="1"/>
-    <row r="523" ht="12.75" customHeight="1"/>
-    <row r="524" ht="12.75" customHeight="1"/>
-    <row r="525" ht="12.75" customHeight="1"/>
-    <row r="526" ht="12.75" customHeight="1"/>
-    <row r="527" ht="12.75" customHeight="1"/>
-    <row r="528" ht="12.75" customHeight="1"/>
-    <row r="529" ht="12.75" customHeight="1"/>
-    <row r="530" ht="12.75" customHeight="1"/>
-    <row r="531" ht="12.75" customHeight="1"/>
-    <row r="532" ht="12.75" customHeight="1"/>
-    <row r="533" ht="12.75" customHeight="1"/>
-    <row r="534" ht="12.75" customHeight="1"/>
-    <row r="535" ht="12.75" customHeight="1"/>
+      <c r="A516" s="2"/>
+      <c r="B516" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="C516" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D516" s="2" t="s">
+        <v>1978</v>
+      </c>
+      <c r="E516" s="2" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="517" ht="12.75" customHeight="1">
+      <c r="B517" s="4" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C517" s="4" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D517" s="4" t="s">
+        <v>1982</v>
+      </c>
+      <c r="E517" s="4" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="518" ht="12.75" customHeight="1">
+      <c r="B518" s="4" t="s">
+        <v>1984</v>
+      </c>
+      <c r="C518" s="4" t="s">
+        <v>1985</v>
+      </c>
+      <c r="D518" s="4" t="s">
+        <v>1986</v>
+      </c>
+      <c r="E518" s="4" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="519" ht="12.75" customHeight="1">
+      <c r="B519" s="4" t="s">
+        <v>1988</v>
+      </c>
+      <c r="C519" s="4" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D519" s="4" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E519" s="4" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="520" ht="12.75" customHeight="1">
+      <c r="B520" s="4" t="s">
+        <v>1992</v>
+      </c>
+      <c r="C520" s="4" t="s">
+        <v>1993</v>
+      </c>
+      <c r="D520" s="4" t="s">
+        <v>1994</v>
+      </c>
+      <c r="E520" s="4" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="521" ht="12.75" customHeight="1">
+      <c r="B521" s="4" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C521" s="4" t="s">
+        <v>1997</v>
+      </c>
+      <c r="D521" s="4" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E521" s="4" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="522" ht="12.75" customHeight="1">
+      <c r="B522" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="C522" s="4" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D522" s="4" t="s">
+        <v>2002</v>
+      </c>
+      <c r="E522" s="4" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="523" ht="12.75" customHeight="1">
+      <c r="B523" s="4" t="s">
+        <v>2004</v>
+      </c>
+      <c r="C523" s="4" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D523" s="4" t="s">
+        <v>2005</v>
+      </c>
+      <c r="E523" s="4" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="524" ht="12.75" customHeight="1">
+      <c r="B524" s="4" t="s">
+        <v>2006</v>
+      </c>
+      <c r="C524" s="4" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D524" s="4" t="s">
+        <v>2008</v>
+      </c>
+      <c r="E524" s="4" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="525" ht="12.75" customHeight="1">
+      <c r="B525" s="4" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C525" s="4" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D525" s="4" t="s">
+        <v>2012</v>
+      </c>
+      <c r="E525" s="4" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="526" ht="12.75" customHeight="1">
+      <c r="B526" s="4" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C526" s="4" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D526" s="4" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E526" s="4" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="527" ht="12.75" customHeight="1">
+      <c r="B527" s="4" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C527" s="4" t="s">
+        <v>2017</v>
+      </c>
+      <c r="D527" s="4" t="s">
+        <v>2017</v>
+      </c>
+      <c r="E527" s="4" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="528" ht="12.75" customHeight="1">
+      <c r="B528" s="4" t="s">
+        <v>2018</v>
+      </c>
+      <c r="C528" s="4" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D528" s="4" t="s">
+        <v>2019</v>
+      </c>
+      <c r="E528" s="4" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="529" ht="12.75" customHeight="1">
+      <c r="B529" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C529" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="D529" s="4" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E529" s="4" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="530" ht="12.75" customHeight="1">
+      <c r="B530" s="13" t="s">
+        <v>2022</v>
+      </c>
+      <c r="C530" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D530" s="4" t="s">
+        <v>2023</v>
+      </c>
+      <c r="E530" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="531" ht="12.75" customHeight="1">
+      <c r="B531" s="13" t="s">
+        <v>2024</v>
+      </c>
+      <c r="C531" s="4" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D531" s="4" t="s">
+        <v>2025</v>
+      </c>
+      <c r="E531" s="4" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="532" ht="12.75" customHeight="1">
+      <c r="B532" s="13" t="s">
+        <v>2026</v>
+      </c>
+      <c r="C532" s="4" t="s">
+        <v>2027</v>
+      </c>
+      <c r="D532" s="4" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E532" s="4" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="533" ht="12.75" customHeight="1">
+      <c r="B533" s="13" t="s">
+        <v>2030</v>
+      </c>
+      <c r="C533" s="4" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D533" s="4" t="s">
+        <v>2032</v>
+      </c>
+      <c r="E533" s="4" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="534" ht="12.75" customHeight="1">
+      <c r="B534" s="13" t="s">
+        <v>2034</v>
+      </c>
+      <c r="C534" s="4" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D534" s="4" t="s">
+        <v>2036</v>
+      </c>
+      <c r="E534" s="4" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="535" ht="12.75" customHeight="1">
+      <c r="B535" s="13" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C535" s="4" t="s">
+        <v>2039</v>
+      </c>
+      <c r="D535" s="4" t="s">
+        <v>2040</v>
+      </c>
+      <c r="E535" s="4" t="s">
+        <v>2041</v>
+      </c>
+    </row>
     <row r="536" ht="12.75" customHeight="1"/>
     <row r="537" ht="12.75" customHeight="1"/>
     <row r="538" ht="12.75" customHeight="1"/>

</xml_diff>